<commit_message>
Updated ITA_grids model - 2025-08-16 11:48
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
+++ b/VerveStacks_ITA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{920C9ACC-3484-4BDC-A431-55BDFBCFEE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{874EEE3F-313B-4385-99B5-D7FF7B0EE2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -776,7 +776,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A827D6A6-DFB6-86A3-8C75-4F5DDEF46EA9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4034E7A1-BDB9-700F-95B3-5BED6A87E9E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>

<commit_message>
Updated ITA_grids model - 2025-08-20 18:31
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
+++ b/VerveStacks_ITA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DD67752-6C9E-4473-B86B-F5DDFFBDEDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{883E15D5-5E95-46BF-8BCB-B9E04446ED4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1902,7 +1902,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9751C492-8175-5303-7CEF-3EFFC846F72D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80F54B3-A4BA-ECB1-EA90-D6A81D910C8C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>

<commit_message>
Updated ITA_grids model - 2025-08-20 18:40
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
+++ b/VerveStacks_ITA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{883E15D5-5E95-46BF-8BCB-B9E04446ED4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7A41C23-F203-4DBD-B2CB-364AC04EC32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1902,7 +1902,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80F54B3-A4BA-ECB1-EA90-D6A81D910C8C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9F1CC5F-F9B3-9695-BB1C-CF46DCA48E83}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>